<commit_message>
Updated Burn Down Chart
</commit_message>
<xml_diff>
--- a/SPSWENG_SystemScape_BurnDownChart_v1.xlsx
+++ b/SPSWENG_SystemScape_BurnDownChart_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="630" windowWidth="19635" windowHeight="7440"/>
+    <workbookView xWindow="720" yWindow="630" windowWidth="10530" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -140,10 +141,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>42052</c:v>
                 </c:pt>
@@ -160,45 +161,39 @@
                   <c:v>42059</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42060</c:v>
+                  <c:v>42061</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42061</c:v>
+                  <c:v>42062</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42062</c:v>
+                  <c:v>42065</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42063</c:v>
+                  <c:v>42066</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42065</c:v>
+                  <c:v>42067</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42066</c:v>
+                  <c:v>42068</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42067</c:v>
+                  <c:v>42069</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42068</c:v>
+                  <c:v>42072</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42069</c:v>
+                  <c:v>42073</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42072</c:v>
+                  <c:v>42074</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42073</c:v>
+                  <c:v>42075</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42074</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42075</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>42076</c:v>
                 </c:pt>
               </c:numCache>
@@ -206,65 +201,59 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$20</c:f>
+              <c:f>Sheet1!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>234</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>221</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>208</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>195</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>182</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>169</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>156</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>143</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>117</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>104</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>91</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>78</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>65</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>52</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>39</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -291,10 +280,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:f>Sheet1!$A$2:$A$18</c:f>
               <c:numCache>
                 <c:formatCode>d\-mmm</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>42052</c:v>
                 </c:pt>
@@ -311,45 +300,39 @@
                   <c:v>42059</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42060</c:v>
+                  <c:v>42061</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42061</c:v>
+                  <c:v>42062</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42062</c:v>
+                  <c:v>42065</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42063</c:v>
+                  <c:v>42066</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42065</c:v>
+                  <c:v>42067</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42066</c:v>
+                  <c:v>42068</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42067</c:v>
+                  <c:v>42069</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42068</c:v>
+                  <c:v>42072</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42069</c:v>
+                  <c:v>42073</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42072</c:v>
+                  <c:v>42074</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42073</c:v>
+                  <c:v>42075</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42074</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>42075</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>42076</c:v>
                 </c:pt>
               </c:numCache>
@@ -357,66 +340,60 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$20</c:f>
+              <c:f>Sheet1!$C$2:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>184</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>181</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>172</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>159</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>159</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>159</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>159</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -433,11 +410,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="69942656"/>
-        <c:axId val="102307712"/>
+        <c:axId val="72543616"/>
+        <c:axId val="72545792"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="69942656"/>
+        <c:axId val="72543616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,14 +443,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102307712"/>
+        <c:crossAx val="72545792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="102307712"/>
+        <c:axId val="72545792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -503,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69942656"/>
+        <c:crossAx val="72543616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -847,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,10 +852,11 @@
         <v>42052</v>
       </c>
       <c r="B2">
-        <v>234</v>
+        <f t="shared" ref="B2:B8" si="0">B3+13</f>
+        <v>208</v>
       </c>
       <c r="C2">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -886,12 +864,12 @@
         <v>42053</v>
       </c>
       <c r="B3">
-        <f>B2-13</f>
-        <v>221</v>
+        <f t="shared" si="0"/>
+        <v>195</v>
       </c>
       <c r="C3">
         <f>C2-3</f>
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,12 +877,12 @@
         <v>42055</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:C20" si="0">B3-13</f>
-        <v>208</v>
+        <f t="shared" si="0"/>
+        <v>182</v>
       </c>
       <c r="C4">
         <f>C3-9</f>
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -913,11 +891,11 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="C5">
-        <f>C4-13</f>
-        <v>159</v>
+        <f>C4-4</f>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,193 +904,166 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:C20" si="1">C5</f>
-        <v>159</v>
+        <f>C5-5</f>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>42060</v>
+        <v>42061</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>169</v>
+        <v>143</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
-        <v>159</v>
+        <f t="shared" ref="C6:C18" si="1">C6</f>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>42061</v>
+        <v>42062</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>42062</v>
+        <v>42065</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>143</v>
+        <f>B10+13</f>
+        <v>117</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>42063</v>
+        <v>42066</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>130</v>
+        <f>B11+13</f>
+        <v>104</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>42065</v>
+        <v>42067</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
-        <v>117</v>
+        <f>B12+13</f>
+        <v>91</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>42066</v>
+        <v>42068</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
-        <v>104</v>
+        <f>B13+13</f>
+        <v>78</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>42067</v>
+        <v>42069</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
-        <v>91</v>
+        <f>B14+13</f>
+        <v>65</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>42068</v>
+        <v>42072</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
-        <v>78</v>
+        <f>B15+13</f>
+        <v>52</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>42069</v>
+        <v>42073</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
-        <v>65</v>
+        <f>B16+13</f>
+        <v>39</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>42072</v>
+        <v>42074</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
-        <v>52</v>
+        <f>B17+13</f>
+        <v>26</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>42073</v>
+        <v>42075</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <f>B18+13</f>
+        <v>13</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>42074</v>
+        <v>42076</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>159</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>42075</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>42076</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Burn Down and SRS
</commit_message>
<xml_diff>
--- a/SPSWENG_SystemScape_BurnDownChart_v1.xlsx
+++ b/SPSWENG_SystemScape_BurnDownChart_v1.xlsx
@@ -387,13 +387,13 @@
                   <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>101</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>101</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>101</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -410,11 +410,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68348160"/>
-        <c:axId val="68350336"/>
+        <c:axId val="68562304"/>
+        <c:axId val="68564480"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="68348160"/>
+        <c:axId val="68562304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,14 +443,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68350336"/>
+        <c:crossAx val="68564480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="68350336"/>
+        <c:axId val="68564480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -480,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68348160"/>
+        <c:crossAx val="68562304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -827,7 +827,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,8 +1037,8 @@
         <v>26</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
-        <v>101</v>
+        <f>C15-90</f>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="C17">
         <f t="shared" si="2"/>
-        <v>101</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="2"/>
-        <v>101</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>